<commit_message>
cập nhật thêm dữ liệu và đổi background đăng nhập
</commit_message>
<xml_diff>
--- a/storage/app/public/data/danhsachduongdung.xlsx
+++ b/storage/app/public/data/danhsachduongdung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\v20\storage\app\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\20V\storage\app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="123">
   <si>
     <t>Mã đường dùng</t>
   </si>
@@ -793,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C564"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
+      <selection activeCell="C525" sqref="C525:C564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -2058,7 +2058,4957 @@
         <v>107</v>
       </c>
       <c r="C114" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="5" t="s">
         <v>2</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C120" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C121" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C123" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C124" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C125" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C127" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C128" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C129" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C130" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C131" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C132" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C133" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C134" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C135" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C136" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C137" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C138" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C139" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C140" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C141" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C142" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C143" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C144" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C145" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C146" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C147" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C148" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C149" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C150" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C151" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C152" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C153" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C154" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C155" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C156" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C157" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A158" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B158" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C158" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C159" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C160" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C161" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C162" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C163" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C164" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C165" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C166" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C167" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C168" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C169" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B170" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C170" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B171" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C171" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C172" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B173" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C173" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C174" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B175" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C175" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B176" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C176" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C177" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B178" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C178" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C179" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C180" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C181" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B182" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C182" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A183" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C183" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C184" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C185" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B186" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C186" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A187" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C187" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A188" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C188" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A189" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C189" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A190" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B190" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C190" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A191" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C191" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A192" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C192" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C193" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C194" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C195" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A196" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C196" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C197" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A198" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C198" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A199" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C199" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A200" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C200" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A201" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C201" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A202" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C202" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A203" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C203" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A204" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C204" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A205" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C205" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A206" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C206" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A207" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C207" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A208" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C208" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A209" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C209" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A210" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C210" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A211" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B211" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C211" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A212" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C212" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A213" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C213" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A214" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C214" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A215" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C215" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A216" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C216" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A217" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B217" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C217" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A218" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C218" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A219" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C219" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A220" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C220" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A221" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C221" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A222" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C222" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A223" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B223" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C223" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A224" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B224" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C224" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A225" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C225" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A226" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C226" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A227" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C227" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A228" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B228" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C228" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A229" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C229" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A230" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C230" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A231" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B231" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C231" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A232" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C232" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A233" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C233" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A234" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B234" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C234" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A235" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B235" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C235" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A236" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B236" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C236" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A237" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B237" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C237" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A238" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B238" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C238" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A239" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B239" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C239" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A240" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B240" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C240" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A241" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B241" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C241" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A242" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B242" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C242" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A243" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B243" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C243" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A244" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B244" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C244" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A245" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B245" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C245" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A246" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B246" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C246" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A247" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B247" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C247" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A248" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C248" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A249" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B249" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C249" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A250" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B250" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C250" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A251" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B251" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C251" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A252" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B252" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C252" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A253" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B253" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C253" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A254" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B254" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C254" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A255" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B255" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C255" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A256" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B256" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C256" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A257" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B257" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C257" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A258" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B258" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C258" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A259" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B259" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C259" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A260" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B260" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C260" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A261" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B261" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C261" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A262" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B262" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C262" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A263" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B263" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C263" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A264" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B264" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C264" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A265" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B265" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C265" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A266" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B266" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C266" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A267" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B267" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C267" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A268" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B268" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C268" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A269" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B269" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C269" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A270" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B270" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C270" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A271" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B271" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C271" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A272" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C272" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A273" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B273" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C273" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A274" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B274" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C274" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A275" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B275" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C275" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A276" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B276" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C276" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A277" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C277" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A278" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C278" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A279" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B279" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C279" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A280" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B280" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C280" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A281" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B281" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C281" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A282" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B282" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C282" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A283" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B283" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C283" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A284" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C284" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A285" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B285" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C285" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A286" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B286" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C286" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A287" s="5">
+        <v>4.05</v>
+      </c>
+      <c r="B287" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C287" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A288" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B288" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C288" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A289" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B289" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C289" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A290" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B290" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C290" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A291" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B291" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C291" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A292" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B292" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C292" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A293" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B293" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C293" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A294" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B294" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C294" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A295" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B295" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C295" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A296" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B296" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C296" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A297" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B297" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C297" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A298" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B298" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C298" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A299" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B299" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C299" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A300" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B300" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C300" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A301" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B301" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C301" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A302" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B302" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C302" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A303" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B303" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C303" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A304" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B304" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C304" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A305" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B305" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C305" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A306" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B306" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C306" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A307" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B307" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C307" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A308" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B308" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C308" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A309" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B309" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C309" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A310" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B310" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C310" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A311" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B311" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C311" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A312" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B312" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C312" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A313" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B313" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C313" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A314" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B314" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C314" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A315" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B315" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C315" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A316" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B316" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C316" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A317" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B317" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C317" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A318" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B318" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C318" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A319" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B319" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C319" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A320" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B320" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C320" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A321" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B321" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C321" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A322" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B322" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C322" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A323" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B323" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C323" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A324" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B324" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C324" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A325" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B325" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C325" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A326" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B326" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C326" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A327" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B327" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C327" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A328" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B328" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C328" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A329" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B329" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C329" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A330" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B330" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C330" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A331" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B331" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C331" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A332" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B332" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C332" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A333" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B333" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C333" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A334" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B334" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C334" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A335" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B335" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C335" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A336" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B336" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C336" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A337" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B337" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C337" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A338" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B338" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C338" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A339" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B339" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C339" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A340" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B340" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C340" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A341" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B341" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C341" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A342" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B342" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C342" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A343" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B343" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C343" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A344" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B344" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C344" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A345" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B345" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C345" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A346" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B346" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C346" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A347" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B347" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C347" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A348" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B348" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C348" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A349" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B349" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C349" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A350" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B350" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C350" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A351" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B351" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C351" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A352" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B352" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C352" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A353" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B353" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C353" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A354" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B354" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C354" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A355" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B355" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C355" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A356" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B356" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C356" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A357" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B357" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C357" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A358" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B358" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C358" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A359" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B359" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C359" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A360" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B360" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C360" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A361" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B361" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C361" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A362" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B362" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C362" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A363" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B363" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C363" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A364" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B364" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C364" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A365" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B365" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C365" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A366" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B366" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C366" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A367" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B367" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C367" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A368" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B368" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C368" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A369" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B369" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C369" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A370" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B370" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C370" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A371" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B371" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C371" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A372" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B372" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C372" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A373" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B373" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C373" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A374" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B374" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C374" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A375" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B375" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C375" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A376" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B376" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C376" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A377" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B377" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C377" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A378" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B378" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C378" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A379" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B379" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C379" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A380" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B380" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C380" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A381" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B381" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C381" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A382" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B382" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C382" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A383" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B383" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C383" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A384" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B384" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C384" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A385" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B385" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C385" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A386" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B386" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C386" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A387" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B387" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C387" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A388" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B388" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C388" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A389" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B389" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C389" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A390" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B390" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C390" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A391" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B391" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C391" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A392" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B392" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C392" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A393" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B393" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C393" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A394" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B394" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C394" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A395" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B395" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C395" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A396" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B396" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C396" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A397" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B397" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C397" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A398" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B398" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C398" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A399" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B399" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C399" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A400" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B400" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C400" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A401" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B401" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C401" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A402" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B402" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C402" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A403" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B403" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C403" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A404" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B404" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C404" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A405" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B405" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C405" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A406" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B406" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C406" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A407" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B407" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C407" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A408" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B408" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C408" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A409" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B409" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C409" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A410" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B410" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C410" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A411" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B411" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C411" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A412" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B412" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C412" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A413" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B413" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C413" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A414" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B414" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C414" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A415" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B415" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C415" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A416" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B416" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C416" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A417" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B417" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C417" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A418" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B418" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C418" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A419" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B419" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C419" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A420" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B420" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C420" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A421" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B421" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C421" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A422" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B422" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C422" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A423" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B423" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C423" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A424" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B424" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C424" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A425" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B425" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C425" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A426" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B426" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C426" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A427" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B427" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C427" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A428" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B428" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C428" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A429" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B429" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C429" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A430" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B430" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C430" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A431" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B431" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C431" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A432" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B432" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C432" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A433" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B433" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C433" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A434" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B434" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C434" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A435" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B435" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C435" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A436" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B436" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C436" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A437" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B437" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C437" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A438" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B438" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C438" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A439" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B439" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C439" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A440" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B440" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C440" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A441" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B441" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C441" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A442" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B442" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C442" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A443" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B443" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C443" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A444" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B444" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C444" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A445" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B445" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C445" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A446" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B446" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C446" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A447" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B447" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C447" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A448" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B448" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C448" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A449" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B449" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C449" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A450" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B450" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C450" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A451" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B451" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C451" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A452" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B452" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C452" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A453" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B453" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C453" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A454" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B454" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C454" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A455" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B455" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C455" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A456" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B456" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C456" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A457" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B457" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C457" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A458" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B458" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C458" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A459" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B459" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C459" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A460" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B460" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C460" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A461" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B461" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C461" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A462" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B462" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C462" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A463" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B463" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C463" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A464" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B464" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C464" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A465" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B465" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C465" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A466" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B466" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C466" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A467" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B467" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C467" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A468" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B468" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C468" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A469" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B469" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C469" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A470" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B470" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C470" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A471" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B471" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C471" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A472" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B472" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C472" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A473" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B473" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C473" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A474" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B474" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C474" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A475" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B475" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C475" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A476" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B476" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C476" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A477" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B477" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C477" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A478" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B478" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C478" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A479" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B479" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C479" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A480" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B480" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C480" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A481" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B481" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C481" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A482" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B482" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C482" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A483" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B483" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C483" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A484" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B484" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C484" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A485" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B485" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C485" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A486" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B486" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C486" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A487" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B487" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C487" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A488" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B488" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C488" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A489" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B489" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C489" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A490" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B490" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C490" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A491" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B491" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C491" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A492" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B492" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C492" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A493" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B493" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C493" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A494" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B494" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C494" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A495" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B495" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C495" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A496" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B496" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C496" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A497" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B497" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C497" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A498" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B498" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C498" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A499" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B499" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C499" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A500" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B500" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C500" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A501" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B501" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C501" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A502" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B502" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C502" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A503" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B503" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C503" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A504" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B504" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C504" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A505" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B505" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C505" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A506" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B506" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C506" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A507" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B507" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C507" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A508" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B508" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C508" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A509" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B509" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C509" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A510" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B510" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C510" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A511" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B511" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C511" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A512" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B512" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C512" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A513" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B513" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C513" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A514" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B514" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C514" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A515" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B515" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C515" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A516" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B516" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C516" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A517" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B517" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C517" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A518" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B518" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C518" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A519" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B519" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C519" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A520" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B520" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C520" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A521" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B521" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C521" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A522" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B522" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C522" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A523" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B523" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C523" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A524" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B524" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C524" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A525" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B525" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C525" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A526" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B526" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C526" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A527" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B527" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C527" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A528" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B528" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C528" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A529" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B529" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C529" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A530" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B530" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C530" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A531" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B531" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C531" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A532" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B532" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C532" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A533" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B533" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C533" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A534" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B534" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C534" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A535" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B535" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C535" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A536" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B536" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C536" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A537" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B537" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C537" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="538" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A538" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B538" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C538" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A539" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B539" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C539" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A540" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B540" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C540" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="541" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A541" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B541" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C541" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A542" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B542" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C542" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A543" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B543" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C543" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A544" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B544" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C544" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A545" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B545" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C545" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="546" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A546" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B546" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C546" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A547" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B547" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C547" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A548" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B548" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C548" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="549" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A549" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B549" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C549" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="550" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A550" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B550" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C550" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A551" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B551" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C551" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="552" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A552" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B552" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C552" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="553" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A553" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B553" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C553" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="554" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A554" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B554" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C554" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="555" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A555" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B555" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C555" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="556" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A556" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B556" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C556" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="557" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A557" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B557" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C557" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A558" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B558" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C558" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="559" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A559" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B559" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C559" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A560" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B560" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C560" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A561" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B561" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C561" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A562" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B562" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C562" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A563" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B563" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C563" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A564" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B564" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C564" s="11">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>